<commit_message>
Mod10: adding hw solution
</commit_message>
<xml_diff>
--- a/mod10/04072015 moon angles rev5a.xlsx
+++ b/mod10/04072015 moon angles rev5a.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\Hopkins\Fall 2018\mod_nav\mod10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="13272" windowHeight="7428"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="13275" windowHeight="7425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>theta 1</t>
   </si>
@@ -89,6 +94,24 @@
   <si>
     <t>8 0 10</t>
   </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>03:00:00</t>
+  </si>
+  <si>
+    <t>06/02/1804</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>38° 36"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -91° 37"</t>
+  </si>
 </sst>
 </file>
 
@@ -150,6 +173,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -241,13 +267,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116577792"/>
-        <c:axId val="155849088"/>
+        <c:axId val="-1238220800"/>
+        <c:axId val="-1067225408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116577792"/>
+        <c:axId val="-1238220800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -256,7 +281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155849088"/>
+        <c:crossAx val="-1067225408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -264,7 +289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155849088"/>
+        <c:axId val="-1067225408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -275,7 +300,148 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116577792"/>
+        <c:crossAx val="-1238220800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$25:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74.478999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.236000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000">
+                  <c:v>74.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>74.433999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74.168000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.085999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.052000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1067230304"/>
+        <c:axId val="-1067227584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1067230304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1067227584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1067227584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1067230304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -301,21 +467,58 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -375,7 +578,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,7 +613,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,27 +827,25 @@
   </sheetPr>
   <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="10.44140625" customWidth="1"/>
-    <col min="20" max="20" width="12.109375" customWidth="1"/>
-    <col min="21" max="21" width="10.5546875" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
-        <v>41353</v>
+        <v>43420</v>
       </c>
       <c r="B1">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -709,82 +910,80 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>31</v>
+        <v>-60</v>
       </c>
       <c r="D3" s="1">
         <f>L3-0.535</f>
-        <v>74.47773861086597</v>
+        <v>94.750130731251204</v>
       </c>
       <c r="E3">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="F3">
-        <f>40.9+1.8-0.1</f>
-        <v>42.599999999999994</v>
+        <v>53</v>
       </c>
       <c r="G3" s="5">
-        <v>84.2</v>
+        <v>56.3</v>
       </c>
       <c r="I3">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="J3">
-        <f>88+0.8-35.6</f>
-        <v>53.199999999999996</v>
+        <v>56.6</v>
       </c>
       <c r="K3">
-        <v>189.3</v>
+        <v>207.7</v>
       </c>
       <c r="L3" s="1">
         <f>R3</f>
-        <v>75.012738610865966</v>
+        <v>95.285130731251201</v>
       </c>
       <c r="N3" s="1">
         <f>E3 + F3/60</f>
-        <v>29.71</v>
+        <v>49.883333333333333</v>
       </c>
       <c r="O3" s="1">
         <f>G3</f>
-        <v>84.2</v>
+        <v>56.3</v>
       </c>
       <c r="P3" s="1">
         <f>I3+J3/60</f>
-        <v>52.886666666666663</v>
+        <v>30.943333333333335</v>
       </c>
       <c r="Q3" s="1">
         <f>K3</f>
-        <v>189.3</v>
+        <v>207.7</v>
       </c>
       <c r="R3" s="1">
         <f>57.3*ACOS(SIN(S3)*SIN(U3)+(COS(S3)*COS(T3)*COS(U3)*COS(V3))+(COS(S3)*SIN(T3)*COS(U3)*SIN(V3)))</f>
-        <v>75.012738610865966</v>
+        <v>95.285130731251201</v>
       </c>
       <c r="S3">
         <f>N3*2*PI()/360</f>
-        <v>0.51853732076751535</v>
+        <v>0.87062840853650481</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:V3" si="0">O3*2*PI()/360</f>
-        <v>1.4695672301792253</v>
+        <v>0.98262036887280746</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>0.92304646373806765</v>
+        <v>0.54006304820877871</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>3.3039082740252659</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+        <v>3.6250488563922221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="D4" s="1"/>
       <c r="G4" s="5"/>
@@ -795,7 +994,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="D5" s="1"/>
       <c r="G5" s="5"/>
@@ -806,86 +1005,82 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>57</v>
+        <v>-60</v>
       </c>
       <c r="D6" s="1">
         <f>L6</f>
-        <v>74.70297637720779</v>
+        <v>93.977130944350179</v>
       </c>
       <c r="E6">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="F6">
-        <f>23.2+1.4-0.1</f>
-        <v>24.499999999999996</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G6" s="5">
-        <f>89.3</f>
-        <v>89.3</v>
+        <v>34.9</v>
       </c>
       <c r="H6"/>
       <c r="I6">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="J6">
-        <f>108.4</f>
-        <v>108.4</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <f>202.8</f>
-        <v>202.8</v>
+        <v>244.9</v>
       </c>
       <c r="L6" s="1">
         <f>R6</f>
-        <v>74.70297637720779</v>
+        <v>93.977130944350179</v>
       </c>
       <c r="M6"/>
       <c r="N6" s="1">
         <f>E6 + F6/60</f>
-        <v>36.408333333333331</v>
+        <v>77.290000000000006</v>
       </c>
       <c r="O6" s="1">
         <f>G6-0.26</f>
-        <v>89.039999999999992</v>
+        <v>34.64</v>
       </c>
       <c r="P6" s="1">
         <f>I6+J6/60</f>
-        <v>51.806666666666665</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="1">
         <f>K6+0.26</f>
-        <v>203.06</v>
+        <v>245.16</v>
       </c>
       <c r="R6" s="1">
         <f>57.3*ACOS(SIN(S6)*SIN(U6)+(COS(S6)*COS(T6)*COS(U6)*COS(V6))+(COS(S6)*SIN(T6)*COS(U6)*SIN(V6)))</f>
-        <v>74.70297637720779</v>
+        <v>93.977130944350179</v>
       </c>
       <c r="S6">
         <f>N6*2*PI()/360</f>
-        <v>0.63544529183026877</v>
+        <v>1.3489649788664173</v>
       </c>
       <c r="T6">
         <f t="shared" ref="T6" si="1">O6*2*PI()/360</f>
-        <v>1.5540411659757507</v>
+        <v>0.60458205289083566</v>
       </c>
       <c r="U6">
         <f t="shared" ref="U6" si="2">P6*2*PI()/360</f>
-        <v>0.90419690781652895</v>
+        <v>0.12217304763960307</v>
       </c>
       <c r="V6">
         <f t="shared" ref="V6" si="3">Q6*2*PI()/360</f>
-        <v>3.5440655790996858</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>4.2788491941892985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -909,7 +1104,7 @@
       <c r="U7"/>
       <c r="V7"/>
     </row>
-    <row r="8" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -933,7 +1128,7 @@
       <c r="U8"/>
       <c r="V8"/>
     </row>
-    <row r="9" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -957,7 +1152,7 @@
       <c r="U9"/>
       <c r="V9"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1219,7 @@
         <v>3.8100537571036215</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1097,7 +1292,7 @@
         <v>2.235766771804736</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>75.119-0.5</f>
         <v>74.619</v>
@@ -1172,7 +1367,7 @@
         <v>2.2404791607851209</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f>D13-0.535</f>
         <v>74.08627783228107</v>
@@ -1245,7 +1440,7 @@
         <v>3.759439208795786</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f>D14-0.535</f>
         <v>73.505986410057531</v>
@@ -1318,7 +1513,7 @@
         <v>3.8170350741115984</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f>D15-0.535</f>
         <v>74.433596167855768</v>
@@ -1391,7 +1586,7 @@
         <v>3.4260813216648689</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <f t="shared" si="4"/>
         <v>75.462025740558076</v>
@@ -1457,7 +1652,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1548,7 +1743,7 @@
       <c r="AH17"/>
       <c r="AI17"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <f t="shared" si="4"/>
         <v>75.849959964428379</v>
@@ -1614,7 +1809,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <f t="shared" si="4"/>
         <v>76.044064826810171</v>
@@ -1680,7 +1875,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <f t="shared" si="4"/>
         <v>76.238259578079763</v>
@@ -1746,7 +1941,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <f t="shared" si="4"/>
         <v>76.432542770152324</v>
@@ -1812,7 +2007,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <f t="shared" si="4"/>
         <v>76.626912963148115</v>
@@ -1878,7 +2073,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <f t="shared" si="4"/>
         <v>76.821368725249783</v>
@@ -1944,7 +2139,7 @@
         <v>3.5395277230445004</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -1952,7 +2147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>0.32097222222222221</v>
       </c>
@@ -1963,7 +2158,7 @@
         <v>74.433999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>0.33344907407407409</v>
       </c>
@@ -1974,7 +2169,7 @@
         <v>74.168000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0.35831018518518515</v>
       </c>
@@ -1985,7 +2180,7 @@
         <v>74.085999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>0.36532407407407402</v>
       </c>
@@ -2005,13 +2200,1415 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1">
+        <f>L3-0.535</f>
+        <v>73.672829802765548</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <f>4.3+14.2</f>
+        <v>18.5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>84.4</v>
+      </c>
+      <c r="I3">
+        <v>53</v>
+      </c>
+      <c r="J3">
+        <f>24+51.1</f>
+        <v>75.099999999999994</v>
+      </c>
+      <c r="K3">
+        <v>190.2</v>
+      </c>
+      <c r="L3" s="1">
+        <f>R3</f>
+        <v>74.207829802765545</v>
+      </c>
+      <c r="N3" s="1">
+        <f>E3 + F3/60</f>
+        <v>30.308333333333334</v>
+      </c>
+      <c r="O3" s="1">
+        <f>G3</f>
+        <v>84.4</v>
+      </c>
+      <c r="P3" s="1">
+        <f>I3+J3/60</f>
+        <v>54.251666666666665</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>K3</f>
+        <v>190.2</v>
+      </c>
+      <c r="R3" s="1">
+        <f>57.3*ACOS(SIN(S3)*SIN(U3)+(COS(S3)*COS(T3)*COS(U3)*COS(V3))+(COS(S3)*SIN(T3)*COS(U3)*SIN(V3)))</f>
+        <v>74.207829802765545</v>
+      </c>
+      <c r="S3">
+        <f>N3*2*PI()/360</f>
+        <v>0.52898020745861474</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:V3" si="0">O3*2*PI()/360</f>
+        <v>1.4730578886832142</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>0.94687020802779032</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="0"/>
+        <v>3.3196162372932148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="G4" s="5"/>
+      <c r="L4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1">
+        <f>L6</f>
+        <v>74.508619069271759</v>
+      </c>
+      <c r="E6">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <f>48.7+14.1</f>
+        <v>62.800000000000004</v>
+      </c>
+      <c r="G6" s="5">
+        <v>84.2</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6">
+        <v>53</v>
+      </c>
+      <c r="J6">
+        <f>26.7+51.1</f>
+        <v>77.8</v>
+      </c>
+      <c r="K6">
+        <v>189.7</v>
+      </c>
+      <c r="L6" s="1">
+        <f>R6</f>
+        <v>74.508619069271759</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6" s="1">
+        <f>E6 + F6/60</f>
+        <v>30.046666666666667</v>
+      </c>
+      <c r="O6" s="1">
+        <f>G6-0.26</f>
+        <v>83.94</v>
+      </c>
+      <c r="P6" s="1">
+        <f>I6+J6/60</f>
+        <v>54.296666666666667</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>K6+0.26</f>
+        <v>189.95999999999998</v>
+      </c>
+      <c r="R6" s="1">
+        <f>57.3*ACOS(SIN(S6)*SIN(U6)+(COS(S6)*COS(T6)*COS(U6)*COS(V6))+(COS(S6)*SIN(T6)*COS(U6)*SIN(V6)))</f>
+        <v>74.508619069271759</v>
+      </c>
+      <c r="S6">
+        <f>N6*2*PI()/360</f>
+        <v>0.52441326258256293</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6:V6" si="1">O6*2*PI()/360</f>
+        <v>1.4650293741240401</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="1"/>
+        <v>0.94765560619118772</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="1"/>
+        <v>3.3154274470884282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7" s="1"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7" s="5"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7" s="1"/>
+      <c r="M7"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+    </row>
+    <row r="8" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8" s="1"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="5"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8" s="1"/>
+      <c r="M8"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+    </row>
+    <row r="9" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9" s="1"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9" s="5"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9" s="1"/>
+      <c r="M9"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10:D23" si="2">L10</f>
+        <v>74.107470264451152</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>5.3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>96.6</v>
+      </c>
+      <c r="I10">
+        <v>47</v>
+      </c>
+      <c r="J10">
+        <v>41.1</v>
+      </c>
+      <c r="K10">
+        <v>218.3</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10:L23" si="3">R10</f>
+        <v>74.107470264451152</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" ref="N10:N23" si="4">E10 + F10/60</f>
+        <v>45.088333333333331</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" ref="O10:O23" si="5">G10</f>
+        <v>96.6</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" ref="P10:P23" si="6">I10+J10/60</f>
+        <v>47.685000000000002</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" ref="Q10:Q23" si="7">K10</f>
+        <v>218.3</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" ref="R10:R23" si="8">57.3*ACOS(SIN(S10)*SIN(U10)+(COS(S10)*COS(T10)*COS(U10)*COS(V10))+(COS(S10)*SIN(T10)*COS(U10)*SIN(V10)))</f>
+        <v>74.107470264451152</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ref="S10:V23" si="9">N10*2*PI()/360</f>
+        <v>0.78693987090337658</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="9"/>
+        <v>1.6859880574265222</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="9"/>
+        <v>0.832260253813496</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="9"/>
+        <v>3.8100537571036215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="2"/>
+        <v>87.879049426190136</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>37.9</v>
+      </c>
+      <c r="G11" s="5">
+        <v>231.3</v>
+      </c>
+      <c r="I11">
+        <v>55</v>
+      </c>
+      <c r="J11">
+        <v>2.9</v>
+      </c>
+      <c r="K11">
+        <v>128.1</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
+        <v>87.879049426190136</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="4"/>
+        <v>11.631666666666666</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="5"/>
+        <v>231.3</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="6"/>
+        <v>55.048333333333332</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="7"/>
+        <v>128.1</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="8"/>
+        <v>87.879049426190136</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="9"/>
+        <v>0.20301088082780708</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="9"/>
+        <v>4.0369465598628844</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="9"/>
+        <v>0.96077466440201187</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="9"/>
+        <v>2.235766771804736</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>75.119-0.5</f>
+        <v>74.619</v>
+      </c>
+      <c r="C12">
+        <v>74.478999999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="2"/>
+        <v>87.749868696869754</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>37.9</v>
+      </c>
+      <c r="G12" s="5">
+        <f>231.3-0.27</f>
+        <v>231.03</v>
+      </c>
+      <c r="I12">
+        <f>54</f>
+        <v>54</v>
+      </c>
+      <c r="J12">
+        <f>62.9-34.2</f>
+        <v>28.699999999999996</v>
+      </c>
+      <c r="K12">
+        <f>128.1+0.27</f>
+        <v>128.37</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="3"/>
+        <v>87.749868696869754</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="4"/>
+        <v>11.631666666666666</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="5"/>
+        <v>231.03</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="6"/>
+        <v>54.478333333333332</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="7"/>
+        <v>128.37</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="8"/>
+        <v>87.749868696869754</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="9"/>
+        <v>0.20301088082780708</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="9"/>
+        <v>4.0322341708825</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="9"/>
+        <v>0.95082628766564403</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="9"/>
+        <v>2.2404791607851209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <f>D13-0.535</f>
+        <v>74.08627783228107</v>
+      </c>
+      <c r="C13">
+        <v>74.236000000000004</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
+        <v>74.621277832281066</v>
+      </c>
+      <c r="E13">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <f>22.5+1.1-0.1</f>
+        <v>23.5</v>
+      </c>
+      <c r="G13" s="5">
+        <v>95.1</v>
+      </c>
+      <c r="I13">
+        <v>48</v>
+      </c>
+      <c r="J13">
+        <f>39+0.9-39.5</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="K13">
+        <v>215.4</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="3"/>
+        <v>74.621277832281066</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="4"/>
+        <v>43.391666666666666</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="5"/>
+        <v>95.1</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="6"/>
+        <v>48.006666666666668</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="7"/>
+        <v>215.4</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="8"/>
+        <v>74.621277832281066</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="9"/>
+        <v>0.75732745126120604</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="9"/>
+        <v>1.6598081186466074</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="9"/>
+        <v>0.83787439624074445</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="9"/>
+        <v>3.759439208795786</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <f>D14-0.535</f>
+        <v>73.505986410057531</v>
+      </c>
+      <c r="C14" s="1">
+        <v>74.2</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>74.040986410057528</v>
+      </c>
+      <c r="E14">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <f>20.3+1-0.1</f>
+        <v>21.2</v>
+      </c>
+      <c r="G14" s="5">
+        <v>96.9</v>
+      </c>
+      <c r="I14">
+        <v>47</v>
+      </c>
+      <c r="J14">
+        <f>32.3+0.9-0.1</f>
+        <v>33.099999999999994</v>
+      </c>
+      <c r="K14">
+        <v>218.7</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="3"/>
+        <v>74.040986410057528</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="4"/>
+        <v>45.353333333333332</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="5"/>
+        <v>96.9</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="6"/>
+        <v>47.551666666666669</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="7"/>
+        <v>218.7</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="8"/>
+        <v>74.040986410057528</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="9"/>
+        <v>0.79156499342116149</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="9"/>
+        <v>1.6912240451825054</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="9"/>
+        <v>0.82993314814417019</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="9"/>
+        <v>3.8170350741115984</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <f>D15-0.535</f>
+        <v>74.433596167855768</v>
+      </c>
+      <c r="C15" s="1">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
+        <v>74.968596167855765</v>
+      </c>
+      <c r="E15">
+        <v>33</v>
+      </c>
+      <c r="F15">
+        <f>4.5+1.5-0.1</f>
+        <v>5.9</v>
+      </c>
+      <c r="G15" s="5">
+        <v>86.7</v>
+      </c>
+      <c r="I15">
+        <v>52</v>
+      </c>
+      <c r="J15">
+        <f>48.5+0.8-36.1</f>
+        <v>13.199999999999996</v>
+      </c>
+      <c r="K15">
+        <v>196.3</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="3"/>
+        <v>74.968596167855765</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="4"/>
+        <v>33.098333333333336</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="5"/>
+        <v>86.7</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="6"/>
+        <v>52.22</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="7"/>
+        <v>196.3</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="8"/>
+        <v>74.968596167855765</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="9"/>
+        <v>0.5776748935892565</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="9"/>
+        <v>1.5132004614790837</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="9"/>
+        <v>0.9114109353914388</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="9"/>
+        <v>3.4260813216648689</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <f t="shared" si="2"/>
+        <v>75.462025740558076</v>
+      </c>
+      <c r="E16">
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F23" si="10">F15-14.5</f>
+        <v>-8.6</v>
+      </c>
+      <c r="G16" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J23" si="11">108.4-52.4</f>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K16">
+        <v>202.8</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="3"/>
+        <v>75.462025740558076</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="4"/>
+        <v>35.856666666666669</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="8"/>
+        <v>75.462025740558076</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="9"/>
+        <v>0.6258168921234335</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <f>C17-0.535</f>
+        <v>74.168000000000006</v>
+      </c>
+      <c r="C17">
+        <v>74.703000000000003</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>75.655946447368322</v>
+      </c>
+      <c r="E17">
+        <v>36</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="10"/>
+        <v>-23.1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17">
+        <v>50</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K17">
+        <v>202.8</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="3"/>
+        <v>75.655946447368322</v>
+      </c>
+      <c r="M17"/>
+      <c r="N17" s="1">
+        <f t="shared" si="4"/>
+        <v>35.615000000000002</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="8"/>
+        <v>75.655946447368322</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="9"/>
+        <v>0.62159901309778043</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>75.849959964428379</v>
+      </c>
+      <c r="E18">
+        <v>36</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="10"/>
+        <v>-37.6</v>
+      </c>
+      <c r="G18" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I18">
+        <v>50</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K18">
+        <v>202.8</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="3"/>
+        <v>75.849959964428379</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="4"/>
+        <v>35.373333333333335</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="8"/>
+        <v>75.849959964428379</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="9"/>
+        <v>0.61738113407212758</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>76.044064826810171</v>
+      </c>
+      <c r="E19">
+        <v>36</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="10"/>
+        <v>-52.1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K19">
+        <v>202.8</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="3"/>
+        <v>76.044064826810171</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="4"/>
+        <v>35.131666666666668</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="8"/>
+        <v>76.044064826810171</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="9"/>
+        <v>0.61316325504647451</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <f t="shared" si="2"/>
+        <v>76.238259578079763</v>
+      </c>
+      <c r="E20">
+        <v>36</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="10"/>
+        <v>-66.599999999999994</v>
+      </c>
+      <c r="G20" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I20">
+        <v>50</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K20">
+        <v>202.8</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="3"/>
+        <v>76.238259578079763</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="4"/>
+        <v>34.89</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="8"/>
+        <v>76.238259578079763</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="9"/>
+        <v>0.60894537602082166</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>76.432542770152324</v>
+      </c>
+      <c r="E21">
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="10"/>
+        <v>-81.099999999999994</v>
+      </c>
+      <c r="G21" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I21">
+        <v>50</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K21">
+        <v>202.8</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="3"/>
+        <v>76.432542770152324</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="4"/>
+        <v>34.648333333333333</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="8"/>
+        <v>76.432542770152324</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="9"/>
+        <v>0.60472749699516859</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>76.626912963148115</v>
+      </c>
+      <c r="E22">
+        <v>36</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="10"/>
+        <v>-95.6</v>
+      </c>
+      <c r="G22" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K22">
+        <v>202.8</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="3"/>
+        <v>76.626912963148115</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="4"/>
+        <v>34.406666666666666</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="8"/>
+        <v>76.626912963148115</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="9"/>
+        <v>0.60050961796951563</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <f t="shared" si="2"/>
+        <v>76.821368725249783</v>
+      </c>
+      <c r="E23">
+        <v>36</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="10"/>
+        <v>-110.1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="I23">
+        <v>50</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="11"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="K23">
+        <v>202.8</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="3"/>
+        <v>76.821368725249783</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="4"/>
+        <v>34.164999999999999</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="5"/>
+        <v>89.3</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="6"/>
+        <v>50.93333333333333</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="7"/>
+        <v>202.8</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" si="8"/>
+        <v>76.821368725249783</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="9"/>
+        <v>0.59629173894386267</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="9"/>
+        <v>1.5585790220309361</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="9"/>
+        <v>0.88895436568244512</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="9"/>
+        <v>3.5395277230445004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0.32097222222222221</v>
+      </c>
+      <c r="B25" s="1">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="C25">
+        <v>74.433999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0.33344907407407409</v>
+      </c>
+      <c r="B26">
+        <v>74.478999999999999</v>
+      </c>
+      <c r="C26">
+        <v>74.168000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.35831018518518515</v>
+      </c>
+      <c r="B27">
+        <v>74.236000000000004</v>
+      </c>
+      <c r="C27">
+        <v>74.085999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>0.36532407407407402</v>
+      </c>
+      <c r="B28" s="1">
+        <v>74.2</v>
+      </c>
+      <c r="C28">
+        <v>74.052000000000007</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="37" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2021,7 +3618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>